<commit_message>
Updated app and readme files for clarity
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E65FBE5-C330-4C82-A4EC-F3F23F953867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DEF9FA-EC67-4F3B-B325-614EE6508273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="1080" windowWidth="16185" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
+    <workbookView xWindow="15150" yWindow="735" windowWidth="13650" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,9 +339,6 @@
     <t>F37</t>
   </si>
   <si>
-    <t xml:space="preserve">If TARGETSPECIES is “YES” the SPECIES must be a target species for the NRMP unless the animal was euthanized then it can be a different species. </t>
-  </si>
-  <si>
     <t>Species issue</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>VNA results issue</t>
+  </si>
+  <si>
+    <t>NRMP target animals are: bobcats, coyotes, foxes, raccoons and skunks.  You have a mismatch between the SPECIES and TARGETSPECIES fields.  Please check to make sure your values are correct for these fields and edit MIS if they are not.</t>
   </si>
 </sst>
 </file>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B3A3A7-3EC3-9D46-96E1-CC6A3D1B7814}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1263,26 +1263,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="C41" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update app with new error codes
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DEF9FA-EC67-4F3B-B325-614EE6508273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2199D6-B086-4E5E-8D9C-15EA6B3B0907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15150" yWindow="735" windowWidth="13650" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
+    <workbookView xWindow="17460" yWindow="2610" windowWidth="10860" windowHeight="11385" xr2:uid="{4719E786-03FF-A74D-9C1B-55BF7F93C6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="106">
   <si>
     <t>F01</t>
   </si>
@@ -246,36 +246,12 @@
     <t>F31</t>
   </si>
   <si>
-    <t>F32</t>
-  </si>
-  <si>
-    <t>DENSITYID should not be filled in when DENSITYSTUDY is “NO”</t>
-  </si>
-  <si>
-    <t>F33</t>
-  </si>
-  <si>
-    <t>You’ve entered a value in OTHERCOLLECTOR but did not choose “OTHER” as COLLECTOR</t>
-  </si>
-  <si>
-    <t>Other collector issue</t>
-  </si>
-  <si>
-    <t>Density study issue</t>
-  </si>
-  <si>
     <t>If COLLECTOR is not “WS” then certain METHOD values and FATE values are not acceptable</t>
   </si>
   <si>
     <t>F34</t>
   </si>
   <si>
-    <t>F35</t>
-  </si>
-  <si>
-    <t>When COLLECTOR is “OTHER”, OTHERCOLLECTOR is a required field</t>
-  </si>
-  <si>
     <t>F36</t>
   </si>
   <si>
@@ -352,13 +328,37 @@
   </si>
   <si>
     <t>NRMP target animals are: bobcats, coyotes, foxes, raccoons and skunks.  You have a mismatch between the SPECIES and TARGETSPECIES fields.  Please check to make sure your values are correct for these fields and edit MIS if they are not.</t>
+  </si>
+  <si>
+    <t>F39</t>
+  </si>
+  <si>
+    <t>F40</t>
+  </si>
+  <si>
+    <t>DAYSPOSTBAIT must be a positive number, check the DATELASTEORV</t>
+  </si>
+  <si>
+    <t>F41</t>
+  </si>
+  <si>
+    <t>F42</t>
+  </si>
+  <si>
+    <t>If ORVNAIVE is "NO" then DATELASTORV must have a value. If ORVNAIVE is "YES" then DATELASTORV must not have a value.</t>
+  </si>
+  <si>
+    <t>If ACTIVITY is "TRAPPING (ORV NAÏVE)" then ORVNAIVE must be "YES" and if ACITIVITY is "TRAPPING (ORV POST-BAIT)" then ORVNAIVE must be "NO"</t>
+  </si>
+  <si>
+    <t>If ORVNAIVE is "YES" then ORVBAITTYPE must be "NONE (NAÏVE)", if ORVNAIVE is "NO" then ORVBAIT type must have a value and cannot be "NONE (NAÏVE)". If ORVBAITYPE is "CS", "FSP", or "ONRAB" then ORVNAIVE must be "NO"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -392,6 +392,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -469,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -494,14 +501,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B3A3A7-3EC3-9D46-96E1-CC6A3D1B7814}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -892,7 +902,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>21</v>
@@ -900,10 +910,10 @@
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>21</v>
@@ -911,10 +921,10 @@
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>21</v>
@@ -1024,7 +1034,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>35</v>
@@ -1035,7 +1045,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>38</v>
@@ -1054,13 +1064,13 @@
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1080,8 +1090,8 @@
       <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>93</v>
+      <c r="B23" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>45</v>
@@ -1092,7 +1102,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>47</v>
@@ -1102,8 +1112,8 @@
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>98</v>
+      <c r="B25" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>49</v>
@@ -1111,13 +1121,13 @@
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1125,7 +1135,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>51</v>
@@ -1135,8 +1145,8 @@
       <c r="A28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>97</v>
+      <c r="B28" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>53</v>
@@ -1210,13 +1220,13 @@
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1227,62 +1237,73 @@
         <v>73</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+    <row r="37" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
+      <c r="C41" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>104</v>
+      <c r="C42" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update to app, new tabs, new user guide
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F88DAD-48E5-4B16-A2D4-DA23BFEDFAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E7C4B1-2669-4148-B9E7-DA33EA18C6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="14955" windowHeight="11385" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t>N32</t>
   </si>
   <si>
-    <t>A tooth sample was taken but it has been &gt;365 days since collection and no age results are entered.  If you have them, please enter results.</t>
-  </si>
-  <si>
     <t>Tooth Results issue</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>N38</t>
+  </si>
+  <si>
+    <t>A tooth sample was taken but it has been &gt;365 days since collection and no age results or TTCC are entered.  If you have them, please enter results.</t>
   </si>
 </sst>
 </file>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B734E-460F-448C-9E99-DEC2DFEF3047}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,73 +1181,73 @@
         <v>83</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="C38" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>82</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="40" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Update app and error codes, allow for .csv files
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30AD589-4B81-4B6B-9D1C-BDA3A373A093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A935E6-A580-4FA8-9CE5-DA45E270EBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1920" windowWidth="14955" windowHeight="11385" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
+    <workbookView xWindow="20625" yWindow="1260" windowWidth="14955" windowHeight="11385" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Please fill in PROCESSED&lt;30DAYSAGO when MISTARGET is “INTENTIONAL” (for trapping).</t>
+  </si>
+  <si>
+    <t>Please fill in RECAPTURE when MISTARGET is “INTENTIONAL” (for trapping).</t>
   </si>
 </sst>
 </file>
@@ -810,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B734E-460F-448C-9E99-DEC2DFEF3047}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1049,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Update app and error N07
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A935E6-A580-4FA8-9CE5-DA45E270EBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37D8A98-B77E-47EC-9B41-F49AADC64141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20625" yWindow="1260" windowWidth="14955" windowHeight="11385" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
+    <workbookView xWindow="17100" yWindow="1260" windowWidth="11700" windowHeight="11385" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -99,9 +99,6 @@
     <t>N07</t>
   </si>
   <si>
-    <t>If METHOD is "HANDCAUGHT/GATHERED" then FATE must be "'DIED UNDER CARE" or "EUTHANIZED" or "FOUND DEAD" or "OTHER" or "RELEASED".  See "scenarios.pdf" (last tab in data checker app).</t>
-  </si>
-  <si>
     <t>N08</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>If METHOD is “WS INCIDENTAL TAKE” then FATE must be “SAMPLED (WS TAKE)”.  See "scenarios.pdf" (last tab in data checker app).</t>
   </si>
   <si>
-    <t>The DATELASTORV you entered doesn’t match the ORV shapefile.  Please check your records and edit in MIS.</t>
-  </si>
-  <si>
     <t>ORV issue</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>Rabies Variant issue</t>
   </si>
   <si>
-    <t>N38</t>
-  </si>
-  <si>
     <t>A tooth sample was taken but it has been &gt;365 days since collection and no age results or TTCC are entered.  If you have them, please enter results.</t>
   </si>
   <si>
@@ -349,6 +340,9 @@
   </si>
   <si>
     <t>Please fill in RECAPTURE when MISTARGET is “INTENTIONAL” (for trapping).</t>
+  </si>
+  <si>
+    <t>If METHOD is "HANDCAUGHT/GATHERED" then FATE must be "'DIED UNDER CARE" or "EUTHANIZED" or "FOUND DEAD" or "RELEASED".  See "scenarios.pdf" (last tab in data checker app).</t>
   </si>
 </sst>
 </file>
@@ -811,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B734E-460F-448C-9E99-DEC2DFEF3047}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>18</v>
@@ -914,10 +908,10 @@
     </row>
     <row r="9" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>18</v>
@@ -925,10 +919,10 @@
     </row>
     <row r="10" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>18</v>
@@ -936,10 +930,10 @@
     </row>
     <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>18</v>
@@ -947,10 +941,10 @@
     </row>
     <row r="12" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>18</v>
@@ -958,10 +952,10 @@
     </row>
     <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>18</v>
@@ -969,10 +963,10 @@
     </row>
     <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>18</v>
@@ -980,288 +974,277 @@
     </row>
     <row r="15" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>34</v>
+      <c r="C39" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update app to check for animals coming back from the dead
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apamydavis\Documents\Rabies\Data checking\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/amy_j_davis_usda_gov/Documents/Documents/Rabies/Data checking/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37D8A98-B77E-47EC-9B41-F49AADC64141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B37D8A98-B77E-47EC-9B41-F49AADC64141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A9D9AC5-00D6-428A-AC43-F3ADC79E131A}"/>
   <bookViews>
-    <workbookView xWindow="17100" yWindow="1260" windowWidth="11700" windowHeight="11385" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="105">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>If METHOD is "HANDCAUGHT/GATHERED" then FATE must be "'DIED UNDER CARE" or "EUTHANIZED" or "FOUND DEAD" or "RELEASED".  See "scenarios.pdf" (last tab in data checker app).</t>
+  </si>
+  <si>
+    <t>N25a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This IDNUMBER has a FATE of "EUTHANIZED" or "FOUND DEAD" or "DIED UNDER CARE" and then is recaptured. Please check your records and edit MIS. </t>
+  </si>
+  <si>
+    <t>ID/Fate issue</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -490,6 +499,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B734E-460F-448C-9E99-DEC2DFEF3047}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C39"/>
+      <selection sqref="A1:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,157 +1105,168 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>57</v>
+        <v>103</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C35" s="12" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+    <row r="40" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C40" s="13" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update app to fix .csv vs .xlsx files
</commit_message>
<xml_diff>
--- a/www/DataCheckingErrorCodes.xlsx
+++ b/www/DataCheckingErrorCodes.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/amy_j_davis_usda_gov/Documents/Documents/Rabies/Data checking/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B37D8A98-B77E-47EC-9B41-F49AADC64141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A9D9AC5-00D6-428A-AC43-F3ADC79E131A}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B37D8A98-B77E-47EC-9B41-F49AADC64141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF10DAED-0D0F-46D9-9234-F8136B1C6C95}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="10110" xr2:uid="{FCDA8828-B151-4A0E-9764-73CEEE176729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$40</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -330,9 +331,6 @@
     <t>You have entered a DATELASTORV, but ORVNAIVE is “YES” or blank. Please check these fields and edit record in MIS.</t>
   </si>
   <si>
-    <t>ORVNAIVE and ORVBAITTYPE do not match; can't have ORV naïve as "YES" or blank with ORV bait and vice versa. Please check these fields and edit record in MIS.</t>
-  </si>
-  <si>
     <t>ORVNAIVE and DATELASTORV do not match; can't have ORV naïve with a Last ORV Date and vice versa.  Please check these fields and edit record in MIS.</t>
   </si>
   <si>
@@ -352,6 +350,9 @@
   </si>
   <si>
     <t>ID/Fate issue</t>
+  </si>
+  <si>
+    <t>ORVNAIVE and ORVBAITTYPE do not match; can't have ORVNAIVE as "YES" or blank with ORVBAITTYPE specified and you can't have ORVNAIVE as "NO" and not provide a ORVBAITTYPE. Please check these fields and edit record in MIS.</t>
   </si>
 </sst>
 </file>
@@ -819,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B734E-460F-448C-9E99-DEC2DFEF3047}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection sqref="A1:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +913,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>18</v>
@@ -1017,12 +1018,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>32</v>
@@ -1033,7 +1034,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>32</v>
@@ -1055,7 +1056,7 @@
         <v>43</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>44</v>
@@ -1066,7 +1067,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>44</v>
@@ -1107,13 +1108,13 @@
     </row>
     <row r="26" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>